<commit_message>
added more results, modifying results and demo merging
</commit_message>
<xml_diff>
--- a/data/north-carolina_results.xlsx
+++ b/data/north-carolina_results.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\terra\democratic_primary_predictions\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Bootcamp\democratic_primary_predictions\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B99F2B5D-98B8-4558-8B39-477D2B242CFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF29D01-A549-4BA3-A297-E0511E8982AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5F3830D1-684C-4DF7-BE6E-0F8A6E54F2A3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="19785" windowHeight="11760" xr2:uid="{5F3830D1-684C-4DF7-BE6E-0F8A6E54F2A3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -384,7 +382,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -393,28 +391,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF666666"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FF666666"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF2A2A2A"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -438,7 +433,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFB264A6"/>
+        <fgColor rgb="FFD18040"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,40 +496,40 @@
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="4" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -850,20 +845,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65341C2F-1787-4683-A124-F17AC0353C4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9F36B11-ECFC-4D70-AAF5-B4C475128099}">
   <dimension ref="A1:P101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:P101"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D107" sqref="D107"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -872,14 +870,14 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>7</v>
@@ -909,30 +907,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5">
-        <v>4346</v>
-      </c>
-      <c r="C2" s="6">
-        <v>7654</v>
-      </c>
-      <c r="D2" s="5">
-        <v>2296</v>
+      <c r="B2" s="6">
+        <v>4383</v>
+      </c>
+      <c r="C2" s="5">
+        <v>7702</v>
+      </c>
+      <c r="D2" s="7">
+        <v>2307</v>
       </c>
       <c r="E2" s="7">
-        <v>1630</v>
+        <v>1646</v>
       </c>
       <c r="F2" s="8">
-        <v>379</v>
+        <v>600</v>
       </c>
       <c r="G2" s="8">
-        <v>600</v>
+        <v>386</v>
       </c>
       <c r="H2" s="8">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="I2" s="8">
         <v>29</v>
@@ -959,27 +957,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="8">
-        <v>431</v>
+      <c r="B3" s="10">
+        <v>435</v>
       </c>
       <c r="C3" s="9">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="D3" s="8">
         <v>430</v>
       </c>
-      <c r="E3" s="10">
-        <v>134</v>
+      <c r="E3" s="8">
+        <v>137</v>
       </c>
       <c r="F3" s="8">
+        <v>87</v>
+      </c>
+      <c r="G3" s="8">
         <v>81</v>
-      </c>
-      <c r="G3" s="8">
-        <v>87</v>
       </c>
       <c r="H3" s="8">
         <v>50</v>
@@ -1009,30 +1007,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="8">
-        <v>207</v>
+      <c r="B4" s="10">
+        <v>210</v>
       </c>
       <c r="C4" s="9">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="D4" s="8">
-        <v>241</v>
-      </c>
-      <c r="E4" s="10">
-        <v>52</v>
+        <v>244</v>
+      </c>
+      <c r="E4" s="8">
+        <v>54</v>
       </c>
       <c r="F4" s="8">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G4" s="8">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="H4" s="8">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="I4" s="8">
         <v>1</v>
@@ -1047,7 +1045,7 @@
         <v>3</v>
       </c>
       <c r="M4" s="8">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="N4" s="8">
         <v>3</v>
@@ -1059,27 +1057,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="10">
         <v>427</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>2070</v>
       </c>
       <c r="D5" s="8">
         <v>364</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="8">
         <v>87</v>
       </c>
       <c r="F5" s="8">
+        <v>32</v>
+      </c>
+      <c r="G5" s="8">
         <v>54</v>
-      </c>
-      <c r="G5" s="8">
-        <v>32</v>
       </c>
       <c r="H5" s="8">
         <v>37</v>
@@ -1109,27 +1107,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="8">
-        <v>528</v>
+      <c r="B6" s="10">
+        <v>536</v>
       </c>
       <c r="C6" s="9">
-        <v>964</v>
+        <v>969</v>
       </c>
       <c r="D6" s="8">
-        <v>373</v>
-      </c>
-      <c r="E6" s="10">
-        <v>229</v>
+        <v>379</v>
+      </c>
+      <c r="E6" s="8">
+        <v>233</v>
       </c>
       <c r="F6" s="8">
+        <v>101</v>
+      </c>
+      <c r="G6" s="8">
         <v>72</v>
-      </c>
-      <c r="G6" s="8">
-        <v>100</v>
       </c>
       <c r="H6" s="8">
         <v>13</v>
@@ -1159,11 +1157,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="10">
         <v>263</v>
       </c>
       <c r="C7" s="9">
@@ -1172,14 +1170,14 @@
       <c r="D7" s="8">
         <v>126</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="8">
         <v>82</v>
       </c>
       <c r="F7" s="8">
+        <v>20</v>
+      </c>
+      <c r="G7" s="8">
         <v>39</v>
-      </c>
-      <c r="G7" s="8">
-        <v>20</v>
       </c>
       <c r="H7" s="8">
         <v>5</v>
@@ -1209,27 +1207,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="10">
         <v>770</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>2752</v>
       </c>
       <c r="D8" s="8">
         <v>876</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>267</v>
       </c>
       <c r="F8" s="8">
+        <v>136</v>
+      </c>
+      <c r="G8" s="8">
         <v>146</v>
-      </c>
-      <c r="G8" s="8">
-        <v>136</v>
       </c>
       <c r="H8" s="8">
         <v>38</v>
@@ -1259,27 +1257,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="10">
         <v>508</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>1794</v>
       </c>
       <c r="D9" s="8">
         <v>459</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="8">
         <v>74</v>
       </c>
       <c r="F9" s="8">
+        <v>29</v>
+      </c>
+      <c r="G9" s="8">
         <v>58</v>
-      </c>
-      <c r="G9" s="8">
-        <v>29</v>
       </c>
       <c r="H9" s="8">
         <v>18</v>
@@ -1309,27 +1307,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="8">
-        <v>578</v>
-      </c>
-      <c r="C10" s="6">
-        <v>2488</v>
+      <c r="B10" s="10">
+        <v>581</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2499</v>
       </c>
       <c r="D10" s="8">
-        <v>511</v>
-      </c>
-      <c r="E10" s="10">
-        <v>136</v>
+        <v>515</v>
+      </c>
+      <c r="E10" s="8">
+        <v>138</v>
       </c>
       <c r="F10" s="8">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="G10" s="8">
-        <v>40</v>
+        <v>72</v>
       </c>
       <c r="H10" s="8">
         <v>42</v>
@@ -1359,27 +1357,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="6">
         <v>2572</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="5">
         <v>7745</v>
       </c>
-      <c r="D11" s="5">
+      <c r="D11" s="7">
         <v>3538</v>
       </c>
       <c r="E11" s="7">
         <v>1076</v>
       </c>
-      <c r="F11" s="8">
+      <c r="F11" s="7">
+        <v>1026</v>
+      </c>
+      <c r="G11" s="8">
         <v>767</v>
-      </c>
-      <c r="G11" s="5">
-        <v>1026</v>
       </c>
       <c r="H11" s="8">
         <v>124</v>
@@ -1409,45 +1407,45 @@
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="11">
-        <v>23227</v>
-      </c>
-      <c r="C12" s="5">
-        <v>15433</v>
-      </c>
-      <c r="D12" s="5">
-        <v>4901</v>
+        <v>23440</v>
+      </c>
+      <c r="C12" s="7">
+        <v>15533</v>
+      </c>
+      <c r="D12" s="7">
+        <v>4928</v>
       </c>
       <c r="E12" s="7">
-        <v>10582</v>
-      </c>
-      <c r="F12" s="5">
-        <v>2383</v>
-      </c>
-      <c r="G12" s="5">
-        <v>3058</v>
-      </c>
-      <c r="H12" s="5">
-        <v>1188</v>
+        <v>10655</v>
+      </c>
+      <c r="F12" s="7">
+        <v>3074</v>
+      </c>
+      <c r="G12" s="7">
+        <v>2397</v>
+      </c>
+      <c r="H12" s="7">
+        <v>1193</v>
       </c>
       <c r="I12" s="8">
         <v>31</v>
       </c>
       <c r="J12" s="8">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="K12" s="8">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="L12" s="8">
         <v>22</v>
       </c>
       <c r="M12" s="8">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="N12" s="8">
         <v>22</v>
@@ -1459,24 +1457,24 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="5">
-        <v>1483</v>
-      </c>
-      <c r="C13" s="6">
-        <v>3007</v>
-      </c>
-      <c r="D13" s="5">
-        <v>1033</v>
-      </c>
-      <c r="E13" s="10">
-        <v>473</v>
+      <c r="B13" s="6">
+        <v>1495</v>
+      </c>
+      <c r="C13" s="5">
+        <v>3026</v>
+      </c>
+      <c r="D13" s="7">
+        <v>1034</v>
+      </c>
+      <c r="E13" s="8">
+        <v>478</v>
       </c>
       <c r="F13" s="8">
-        <v>221</v>
+        <v>229</v>
       </c>
       <c r="G13" s="8">
         <v>224</v>
@@ -1506,30 +1504,30 @@
         <v>5</v>
       </c>
       <c r="P13" s="8">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="6">
         <v>5285</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>10585</v>
       </c>
-      <c r="D14" s="5">
+      <c r="D14" s="7">
         <v>2335</v>
       </c>
       <c r="E14" s="7">
         <v>1656</v>
       </c>
       <c r="F14" s="8">
+        <v>387</v>
+      </c>
+      <c r="G14" s="8">
         <v>274</v>
-      </c>
-      <c r="G14" s="8">
-        <v>387</v>
       </c>
       <c r="H14" s="8">
         <v>108</v>
@@ -1559,27 +1557,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="6">
         <v>1036</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>1849</v>
       </c>
       <c r="D15" s="8">
         <v>680</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <v>297</v>
       </c>
       <c r="F15" s="8">
+        <v>186</v>
+      </c>
+      <c r="G15" s="8">
         <v>116</v>
-      </c>
-      <c r="G15" s="8">
-        <v>186</v>
       </c>
       <c r="H15" s="8">
         <v>39</v>
@@ -1609,11 +1607,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="10">
         <v>116</v>
       </c>
       <c r="C16" s="9">
@@ -1622,14 +1620,14 @@
       <c r="D16" s="8">
         <v>125</v>
       </c>
-      <c r="E16" s="10">
+      <c r="E16" s="8">
         <v>53</v>
       </c>
       <c r="F16" s="8">
+        <v>29</v>
+      </c>
+      <c r="G16" s="8">
         <v>13</v>
-      </c>
-      <c r="G16" s="8">
-        <v>29</v>
       </c>
       <c r="H16" s="8">
         <v>4</v>
@@ -1659,27 +1657,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="6">
         <v>1237</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="5">
         <v>2948</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="7">
         <v>1231</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E17" s="8">
         <v>497</v>
       </c>
       <c r="F17" s="8">
+        <v>286</v>
+      </c>
+      <c r="G17" s="8">
         <v>242</v>
-      </c>
-      <c r="G17" s="8">
-        <v>286</v>
       </c>
       <c r="H17" s="8">
         <v>57</v>
@@ -1709,27 +1707,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="8">
-        <v>566</v>
-      </c>
-      <c r="C18" s="6">
-        <v>1469</v>
+      <c r="B18" s="10">
+        <v>569</v>
+      </c>
+      <c r="C18" s="5">
+        <v>1473</v>
       </c>
       <c r="D18" s="8">
         <v>476</v>
       </c>
-      <c r="E18" s="10">
-        <v>142</v>
+      <c r="E18" s="8">
+        <v>143</v>
       </c>
       <c r="F18" s="8">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="G18" s="8">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="H18" s="8">
         <v>27</v>
@@ -1759,27 +1757,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B19" s="5">
-        <v>2745</v>
-      </c>
-      <c r="C19" s="6">
-        <v>4596</v>
-      </c>
-      <c r="D19" s="5">
-        <v>1731</v>
-      </c>
-      <c r="E19" s="10">
-        <v>863</v>
+      <c r="B19" s="6">
+        <v>2775</v>
+      </c>
+      <c r="C19" s="5">
+        <v>4618</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1732</v>
+      </c>
+      <c r="E19" s="8">
+        <v>876</v>
       </c>
       <c r="F19" s="8">
-        <v>309</v>
+        <v>502</v>
       </c>
       <c r="G19" s="8">
-        <v>498</v>
+        <v>312</v>
       </c>
       <c r="H19" s="8">
         <v>94</v>
@@ -1809,27 +1807,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="5">
-        <v>3382</v>
-      </c>
-      <c r="C20" s="6">
-        <v>6408</v>
-      </c>
-      <c r="D20" s="5">
-        <v>2788</v>
+      <c r="B20" s="6">
+        <v>3408</v>
+      </c>
+      <c r="C20" s="5">
+        <v>6455</v>
+      </c>
+      <c r="D20" s="7">
+        <v>2794</v>
       </c>
       <c r="E20" s="7">
-        <v>2375</v>
+        <v>2388</v>
       </c>
       <c r="F20" s="8">
-        <v>696</v>
+        <v>845</v>
       </c>
       <c r="G20" s="8">
-        <v>843</v>
+        <v>700</v>
       </c>
       <c r="H20" s="8">
         <v>103</v>
@@ -1838,7 +1836,7 @@
         <v>17</v>
       </c>
       <c r="J20" s="8">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="K20" s="8">
         <v>38</v>
@@ -1859,27 +1857,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B21" s="8">
-        <v>441</v>
+      <c r="B21" s="10">
+        <v>446</v>
       </c>
       <c r="C21" s="9">
-        <v>823</v>
+        <v>831</v>
       </c>
       <c r="D21" s="8">
         <v>246</v>
       </c>
-      <c r="E21" s="10">
-        <v>139</v>
+      <c r="E21" s="8">
+        <v>140</v>
       </c>
       <c r="F21" s="8">
+        <v>66</v>
+      </c>
+      <c r="G21" s="8">
         <v>55</v>
-      </c>
-      <c r="G21" s="8">
-        <v>65</v>
       </c>
       <c r="H21" s="8">
         <v>21</v>
@@ -1888,7 +1886,7 @@
         <v>3</v>
       </c>
       <c r="J21" s="8">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="K21" s="8">
         <v>10</v>
@@ -1909,27 +1907,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B22" s="8">
-        <v>180</v>
+      <c r="B22" s="10">
+        <v>184</v>
       </c>
       <c r="C22" s="9">
-        <v>827</v>
+        <v>831</v>
       </c>
       <c r="D22" s="8">
-        <v>273</v>
-      </c>
-      <c r="E22" s="10">
+        <v>275</v>
+      </c>
+      <c r="E22" s="8">
         <v>78</v>
       </c>
       <c r="F22" s="8">
+        <v>45</v>
+      </c>
+      <c r="G22" s="8">
         <v>36</v>
-      </c>
-      <c r="G22" s="8">
-        <v>45</v>
       </c>
       <c r="H22" s="8">
         <v>9</v>
@@ -1950,29 +1948,29 @@
         <v>5</v>
       </c>
       <c r="N22" s="8">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O22" s="8">
         <v>6</v>
       </c>
       <c r="P22" s="8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="8">
-        <v>200</v>
+      <c r="B23" s="10">
+        <v>201</v>
       </c>
       <c r="C23" s="9">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D23" s="8">
         <v>130</v>
       </c>
-      <c r="E23" s="10">
+      <c r="E23" s="8">
         <v>92</v>
       </c>
       <c r="F23" s="8">
@@ -2000,7 +1998,7 @@
         <v>6</v>
       </c>
       <c r="N23" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O23" s="8">
         <v>1</v>
@@ -2009,27 +2007,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="5">
-        <v>1392</v>
-      </c>
-      <c r="C24" s="6">
-        <v>4185</v>
-      </c>
-      <c r="D24" s="5">
-        <v>1247</v>
-      </c>
-      <c r="E24" s="10">
-        <v>420</v>
+      <c r="B24" s="6">
+        <v>1406</v>
+      </c>
+      <c r="C24" s="5">
+        <v>4197</v>
+      </c>
+      <c r="D24" s="7">
+        <v>1250</v>
+      </c>
+      <c r="E24" s="8">
+        <v>424</v>
       </c>
       <c r="F24" s="8">
+        <v>132</v>
+      </c>
+      <c r="G24" s="8">
         <v>174</v>
-      </c>
-      <c r="G24" s="8">
-        <v>131</v>
       </c>
       <c r="H24" s="8">
         <v>81</v>
@@ -2038,7 +2036,7 @@
         <v>16</v>
       </c>
       <c r="J24" s="8">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K24" s="8">
         <v>16</v>
@@ -2059,30 +2057,30 @@
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B25" s="8">
-        <v>826</v>
-      </c>
-      <c r="C25" s="6">
-        <v>2555</v>
+      <c r="B25" s="10">
+        <v>832</v>
+      </c>
+      <c r="C25" s="5">
+        <v>2566</v>
       </c>
       <c r="D25" s="8">
-        <v>522</v>
-      </c>
-      <c r="E25" s="10">
-        <v>196</v>
+        <v>525</v>
+      </c>
+      <c r="E25" s="8">
+        <v>197</v>
       </c>
       <c r="F25" s="8">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="G25" s="8">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="H25" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="I25" s="8">
         <v>21</v>
@@ -2100,7 +2098,7 @@
         <v>21</v>
       </c>
       <c r="N25" s="8">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="O25" s="8">
         <v>21</v>
@@ -2109,30 +2107,30 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B26" s="5">
-        <v>1737</v>
-      </c>
-      <c r="C26" s="6">
-        <v>5085</v>
-      </c>
-      <c r="D26" s="5">
-        <v>1887</v>
-      </c>
-      <c r="E26" s="10">
-        <v>562</v>
+      <c r="B26" s="6">
+        <v>1748</v>
+      </c>
+      <c r="C26" s="5">
+        <v>5100</v>
+      </c>
+      <c r="D26" s="7">
+        <v>1894</v>
+      </c>
+      <c r="E26" s="8">
+        <v>565</v>
       </c>
       <c r="F26" s="8">
+        <v>391</v>
+      </c>
+      <c r="G26" s="8">
         <v>301</v>
       </c>
-      <c r="G26" s="8">
-        <v>390</v>
-      </c>
       <c r="H26" s="8">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="I26" s="8">
         <v>19</v>
@@ -2147,7 +2145,7 @@
         <v>2</v>
       </c>
       <c r="M26" s="8">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="N26" s="8">
         <v>10</v>
@@ -2159,30 +2157,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B27" s="5">
-        <v>7334</v>
-      </c>
-      <c r="C27" s="6">
-        <v>19482</v>
-      </c>
-      <c r="D27" s="5">
-        <v>4801</v>
+      <c r="B27" s="6">
+        <v>7393</v>
+      </c>
+      <c r="C27" s="5">
+        <v>19559</v>
+      </c>
+      <c r="D27" s="7">
+        <v>4822</v>
       </c>
       <c r="E27" s="7">
-        <v>1905</v>
+        <v>1921</v>
       </c>
       <c r="F27" s="8">
-        <v>372</v>
+        <v>533</v>
       </c>
       <c r="G27" s="8">
-        <v>530</v>
+        <v>373</v>
       </c>
       <c r="H27" s="8">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="I27" s="8">
         <v>103</v>
@@ -2197,39 +2195,39 @@
         <v>28</v>
       </c>
       <c r="M27" s="8">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="N27" s="8">
         <v>27</v>
       </c>
       <c r="O27" s="8">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="P27" s="8">
         <v>35</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B28" s="8">
-        <v>419</v>
+      <c r="B28" s="10">
+        <v>427</v>
       </c>
       <c r="C28" s="9">
-        <v>952</v>
+        <v>960</v>
       </c>
       <c r="D28" s="8">
-        <v>274</v>
-      </c>
-      <c r="E28" s="10">
-        <v>170</v>
+        <v>276</v>
+      </c>
+      <c r="E28" s="8">
+        <v>171</v>
       </c>
       <c r="F28" s="8">
+        <v>54</v>
+      </c>
+      <c r="G28" s="8">
         <v>36</v>
-      </c>
-      <c r="G28" s="8">
-        <v>54</v>
       </c>
       <c r="H28" s="8">
         <v>8</v>
@@ -2259,27 +2257,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B29" s="5">
+      <c r="B29" s="6">
         <v>1267</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="5">
         <v>2167</v>
       </c>
       <c r="D29" s="8">
         <v>779</v>
       </c>
-      <c r="E29" s="10">
+      <c r="E29" s="8">
         <v>507</v>
       </c>
       <c r="F29" s="8">
+        <v>231</v>
+      </c>
+      <c r="G29" s="8">
         <v>153</v>
-      </c>
-      <c r="G29" s="8">
-        <v>231</v>
       </c>
       <c r="H29" s="8">
         <v>26</v>
@@ -2309,27 +2307,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="5">
+      <c r="B30" s="6">
         <v>2194</v>
       </c>
-      <c r="C30" s="6">
+      <c r="C30" s="5">
         <v>4367</v>
       </c>
-      <c r="D30" s="5">
+      <c r="D30" s="7">
         <v>1482</v>
       </c>
-      <c r="E30" s="10">
+      <c r="E30" s="8">
         <v>559</v>
       </c>
       <c r="F30" s="8">
+        <v>337</v>
+      </c>
+      <c r="G30" s="8">
         <v>279</v>
-      </c>
-      <c r="G30" s="8">
-        <v>337</v>
       </c>
       <c r="H30" s="8">
         <v>64</v>
@@ -2359,27 +2357,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="8">
-        <v>697</v>
-      </c>
-      <c r="C31" s="6">
-        <v>1266</v>
+      <c r="B31" s="10">
+        <v>706</v>
+      </c>
+      <c r="C31" s="5">
+        <v>1275</v>
       </c>
       <c r="D31" s="8">
-        <v>550</v>
-      </c>
-      <c r="E31" s="10">
-        <v>236</v>
+        <v>552</v>
+      </c>
+      <c r="E31" s="8">
+        <v>238</v>
       </c>
       <c r="F31" s="8">
+        <v>133</v>
+      </c>
+      <c r="G31" s="8">
         <v>118</v>
-      </c>
-      <c r="G31" s="8">
-        <v>133</v>
       </c>
       <c r="H31" s="8">
         <v>21</v>
@@ -2409,27 +2407,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="8">
+      <c r="B32" s="10">
         <v>672</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="5">
         <v>2477</v>
       </c>
       <c r="D32" s="8">
         <v>685</v>
       </c>
-      <c r="E32" s="10">
+      <c r="E32" s="8">
         <v>133</v>
       </c>
       <c r="F32" s="8">
+        <v>45</v>
+      </c>
+      <c r="G32" s="8">
         <v>82</v>
-      </c>
-      <c r="G32" s="8">
-        <v>45</v>
       </c>
       <c r="H32" s="8">
         <v>24</v>
@@ -2459,27 +2457,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="33" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B33" s="5">
+      <c r="B33" s="6">
         <v>21759</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="5">
         <v>29324</v>
       </c>
-      <c r="D33" s="5">
+      <c r="D33" s="7">
         <v>7439</v>
       </c>
       <c r="E33" s="7">
         <v>16408</v>
       </c>
-      <c r="F33" s="5">
+      <c r="F33" s="7">
+        <v>2889</v>
+      </c>
+      <c r="G33" s="7">
         <v>1792</v>
-      </c>
-      <c r="G33" s="5">
-        <v>2889</v>
       </c>
       <c r="H33" s="8">
         <v>260</v>
@@ -2509,27 +2507,27 @@
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="5">
-        <v>1035</v>
-      </c>
-      <c r="C34" s="6">
-        <v>3973</v>
-      </c>
-      <c r="D34" s="5">
-        <v>1193</v>
-      </c>
-      <c r="E34" s="10">
-        <v>250</v>
+      <c r="B34" s="6">
+        <v>1043</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3982</v>
+      </c>
+      <c r="D34" s="7">
+        <v>1198</v>
+      </c>
+      <c r="E34" s="8">
+        <v>252</v>
       </c>
       <c r="F34" s="8">
+        <v>73</v>
+      </c>
+      <c r="G34" s="8">
         <v>80</v>
-      </c>
-      <c r="G34" s="8">
-        <v>72</v>
       </c>
       <c r="H34" s="8">
         <v>44</v>
@@ -2538,7 +2536,7 @@
         <v>25</v>
       </c>
       <c r="J34" s="8">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="K34" s="8">
         <v>16</v>
@@ -2559,27 +2557,27 @@
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="5">
-        <v>14114</v>
-      </c>
-      <c r="C35" s="6">
-        <v>23689</v>
-      </c>
-      <c r="D35" s="5">
-        <v>7739</v>
+      <c r="B35" s="6">
+        <v>14296</v>
+      </c>
+      <c r="C35" s="5">
+        <v>23929</v>
+      </c>
+      <c r="D35" s="7">
+        <v>7797</v>
       </c>
       <c r="E35" s="7">
-        <v>5236</v>
-      </c>
-      <c r="F35" s="5">
-        <v>1148</v>
-      </c>
-      <c r="G35" s="5">
-        <v>2146</v>
+        <v>5307</v>
+      </c>
+      <c r="F35" s="7">
+        <v>2166</v>
+      </c>
+      <c r="G35" s="7">
+        <v>1152</v>
       </c>
       <c r="H35" s="8">
         <v>203</v>
@@ -2588,48 +2586,48 @@
         <v>109</v>
       </c>
       <c r="J35" s="8">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="K35" s="8">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="L35" s="8">
         <v>29</v>
       </c>
       <c r="M35" s="8">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="N35" s="8">
         <v>27</v>
       </c>
       <c r="O35" s="8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="P35" s="8">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B36" s="5">
-        <v>1578</v>
-      </c>
-      <c r="C36" s="6">
-        <v>3728</v>
-      </c>
-      <c r="D36" s="5">
-        <v>1217</v>
-      </c>
-      <c r="E36" s="10">
+      <c r="B36" s="6">
+        <v>1581</v>
+      </c>
+      <c r="C36" s="5">
+        <v>3733</v>
+      </c>
+      <c r="D36" s="7">
+        <v>1218</v>
+      </c>
+      <c r="E36" s="8">
         <v>496</v>
       </c>
       <c r="F36" s="8">
+        <v>189</v>
+      </c>
+      <c r="G36" s="8">
         <v>460</v>
-      </c>
-      <c r="G36" s="8">
-        <v>189</v>
       </c>
       <c r="H36" s="8">
         <v>51</v>
@@ -2659,39 +2657,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="5">
-        <v>3992</v>
-      </c>
-      <c r="C37" s="6">
-        <v>7874</v>
-      </c>
-      <c r="D37" s="5">
-        <v>2146</v>
+      <c r="B37" s="6">
+        <v>4043</v>
+      </c>
+      <c r="C37" s="5">
+        <v>7920</v>
+      </c>
+      <c r="D37" s="7">
+        <v>2159</v>
       </c>
       <c r="E37" s="7">
-        <v>1190</v>
+        <v>1207</v>
       </c>
       <c r="F37" s="8">
+        <v>478</v>
+      </c>
+      <c r="G37" s="8">
         <v>345</v>
-      </c>
-      <c r="G37" s="8">
-        <v>476</v>
       </c>
       <c r="H37" s="8">
         <v>146</v>
       </c>
       <c r="I37" s="8">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J37" s="8">
         <v>89</v>
       </c>
       <c r="K37" s="8">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="L37" s="8">
         <v>10</v>
@@ -2700,7 +2698,7 @@
         <v>23</v>
       </c>
       <c r="N37" s="8">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="O37" s="8">
         <v>16</v>
@@ -2709,11 +2707,11 @@
         <v>27</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B38" s="8">
+      <c r="B38" s="10">
         <v>219</v>
       </c>
       <c r="C38" s="9">
@@ -2722,14 +2720,14 @@
       <c r="D38" s="8">
         <v>224</v>
       </c>
-      <c r="E38" s="10">
+      <c r="E38" s="8">
         <v>71</v>
       </c>
       <c r="F38" s="8">
+        <v>15</v>
+      </c>
+      <c r="G38" s="8">
         <v>25</v>
-      </c>
-      <c r="G38" s="8">
-        <v>15</v>
       </c>
       <c r="H38" s="8">
         <v>10</v>
@@ -2759,27 +2757,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="39" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B39" s="8">
+      <c r="B39" s="10">
         <v>97</v>
       </c>
       <c r="C39" s="9">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="D39" s="8">
         <v>69</v>
       </c>
-      <c r="E39" s="10">
+      <c r="E39" s="8">
         <v>33</v>
       </c>
       <c r="F39" s="8">
+        <v>12</v>
+      </c>
+      <c r="G39" s="8">
         <v>28</v>
-      </c>
-      <c r="G39" s="8">
-        <v>12</v>
       </c>
       <c r="H39" s="8">
         <v>29</v>
@@ -2809,27 +2807,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B40" s="5">
-        <v>1578</v>
-      </c>
-      <c r="C40" s="6">
-        <v>3457</v>
-      </c>
-      <c r="D40" s="5">
-        <v>1056</v>
-      </c>
-      <c r="E40" s="10">
-        <v>470</v>
+      <c r="B40" s="6">
+        <v>1583</v>
+      </c>
+      <c r="C40" s="5">
+        <v>3472</v>
+      </c>
+      <c r="D40" s="7">
+        <v>1062</v>
+      </c>
+      <c r="E40" s="8">
+        <v>471</v>
       </c>
       <c r="F40" s="8">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="G40" s="8">
-        <v>218</v>
+        <v>192</v>
       </c>
       <c r="H40" s="8">
         <v>55</v>
@@ -2838,7 +2836,7 @@
         <v>17</v>
       </c>
       <c r="J40" s="8">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="K40" s="8">
         <v>17</v>
@@ -2859,27 +2857,27 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="B41" s="8">
+      <c r="B41" s="10">
         <v>417</v>
       </c>
-      <c r="C41" s="6">
-        <v>1093</v>
+      <c r="C41" s="5">
+        <v>1098</v>
       </c>
       <c r="D41" s="8">
-        <v>314</v>
-      </c>
-      <c r="E41" s="10">
+        <v>315</v>
+      </c>
+      <c r="E41" s="8">
         <v>82</v>
       </c>
       <c r="F41" s="8">
+        <v>19</v>
+      </c>
+      <c r="G41" s="8">
         <v>52</v>
-      </c>
-      <c r="G41" s="8">
-        <v>19</v>
       </c>
       <c r="H41" s="8">
         <v>31</v>
@@ -2909,27 +2907,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="B42" s="5">
-        <v>21196</v>
-      </c>
-      <c r="C42" s="6">
-        <v>37288</v>
-      </c>
-      <c r="D42" s="5">
-        <v>10246</v>
+      <c r="B42" s="6">
+        <v>21337</v>
+      </c>
+      <c r="C42" s="5">
+        <v>37425</v>
+      </c>
+      <c r="D42" s="7">
+        <v>10288</v>
       </c>
       <c r="E42" s="7">
-        <v>7419</v>
-      </c>
-      <c r="F42" s="5">
-        <v>1379</v>
-      </c>
-      <c r="G42" s="5">
-        <v>2194</v>
+        <v>7491</v>
+      </c>
+      <c r="F42" s="7">
+        <v>2205</v>
+      </c>
+      <c r="G42" s="7">
+        <v>1396</v>
       </c>
       <c r="H42" s="8">
         <v>298</v>
@@ -2941,7 +2939,7 @@
         <v>251</v>
       </c>
       <c r="K42" s="8">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="L42" s="8">
         <v>39</v>
@@ -2950,7 +2948,7 @@
         <v>131</v>
       </c>
       <c r="N42" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O42" s="8">
         <v>63</v>
@@ -2959,27 +2957,27 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B43" s="5">
+      <c r="B43" s="6">
         <v>1127</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="5">
         <v>4830</v>
       </c>
       <c r="D43" s="8">
         <v>882</v>
       </c>
-      <c r="E43" s="10">
+      <c r="E43" s="8">
         <v>255</v>
       </c>
       <c r="F43" s="8">
+        <v>71</v>
+      </c>
+      <c r="G43" s="8">
         <v>103</v>
-      </c>
-      <c r="G43" s="8">
-        <v>71</v>
       </c>
       <c r="H43" s="8">
         <v>32</v>
@@ -3009,27 +3007,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="B44" s="5">
-        <v>1895</v>
-      </c>
-      <c r="C44" s="6">
-        <v>4281</v>
-      </c>
-      <c r="D44" s="5">
-        <v>1149</v>
-      </c>
-      <c r="E44" s="10">
-        <v>536</v>
+      <c r="B44" s="6">
+        <v>1924</v>
+      </c>
+      <c r="C44" s="5">
+        <v>4324</v>
+      </c>
+      <c r="D44" s="7">
+        <v>1157</v>
+      </c>
+      <c r="E44" s="8">
+        <v>541</v>
       </c>
       <c r="F44" s="8">
-        <v>155</v>
+        <v>218</v>
       </c>
       <c r="G44" s="8">
-        <v>214</v>
+        <v>157</v>
       </c>
       <c r="H44" s="8">
         <v>61</v>
@@ -3038,10 +3036,10 @@
         <v>25</v>
       </c>
       <c r="J44" s="8">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K44" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="L44" s="8">
         <v>5</v>
@@ -3059,27 +3057,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="B45" s="5">
+      <c r="B45" s="6">
         <v>1940</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="5">
         <v>3444</v>
       </c>
       <c r="D45" s="8">
         <v>846</v>
       </c>
-      <c r="E45" s="10">
+      <c r="E45" s="8">
         <v>767</v>
       </c>
       <c r="F45" s="8">
+        <v>381</v>
+      </c>
+      <c r="G45" s="8">
         <v>356</v>
-      </c>
-      <c r="G45" s="8">
-        <v>381</v>
       </c>
       <c r="H45" s="8">
         <v>352</v>
@@ -3109,30 +3107,30 @@
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="B46" s="5">
-        <v>3709</v>
-      </c>
-      <c r="C46" s="6">
-        <v>5678</v>
-      </c>
-      <c r="D46" s="5">
-        <v>1581</v>
+      <c r="B46" s="6">
+        <v>3729</v>
+      </c>
+      <c r="C46" s="5">
+        <v>5713</v>
+      </c>
+      <c r="D46" s="7">
+        <v>1588</v>
       </c>
       <c r="E46" s="7">
-        <v>1633</v>
+        <v>1641</v>
       </c>
       <c r="F46" s="8">
-        <v>694</v>
+        <v>866</v>
       </c>
       <c r="G46" s="8">
-        <v>861</v>
+        <v>698</v>
       </c>
       <c r="H46" s="8">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="I46" s="8">
         <v>8</v>
@@ -3159,27 +3157,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="B47" s="8">
-        <v>432</v>
-      </c>
-      <c r="C47" s="6">
-        <v>2373</v>
+      <c r="B47" s="10">
+        <v>433</v>
+      </c>
+      <c r="C47" s="5">
+        <v>2377</v>
       </c>
       <c r="D47" s="8">
         <v>534</v>
       </c>
-      <c r="E47" s="10">
-        <v>102</v>
+      <c r="E47" s="8">
+        <v>103</v>
       </c>
       <c r="F47" s="8">
+        <v>32</v>
+      </c>
+      <c r="G47" s="8">
         <v>44</v>
-      </c>
-      <c r="G47" s="8">
-        <v>32</v>
       </c>
       <c r="H47" s="8">
         <v>11</v>
@@ -3209,27 +3207,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="B48" s="5">
-        <v>1112</v>
-      </c>
-      <c r="C48" s="6">
-        <v>2797</v>
+      <c r="B48" s="6">
+        <v>1114</v>
+      </c>
+      <c r="C48" s="5">
+        <v>2801</v>
       </c>
       <c r="D48" s="8">
         <v>648</v>
       </c>
-      <c r="E48" s="10">
+      <c r="E48" s="8">
         <v>215</v>
       </c>
       <c r="F48" s="8">
+        <v>68</v>
+      </c>
+      <c r="G48" s="8">
         <v>55</v>
-      </c>
-      <c r="G48" s="8">
-        <v>68</v>
       </c>
       <c r="H48" s="8">
         <v>39</v>
@@ -3259,11 +3257,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="B49" s="8">
+      <c r="B49" s="10">
         <v>127</v>
       </c>
       <c r="C49" s="9">
@@ -3272,14 +3270,14 @@
       <c r="D49" s="8">
         <v>86</v>
       </c>
-      <c r="E49" s="10">
+      <c r="E49" s="8">
         <v>83</v>
       </c>
       <c r="F49" s="8">
+        <v>7</v>
+      </c>
+      <c r="G49" s="8">
         <v>23</v>
-      </c>
-      <c r="G49" s="8">
-        <v>7</v>
       </c>
       <c r="H49" s="8">
         <v>10</v>
@@ -3309,30 +3307,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="B50" s="5">
-        <v>3383</v>
-      </c>
-      <c r="C50" s="6">
-        <v>6210</v>
-      </c>
-      <c r="D50" s="5">
-        <v>2496</v>
+      <c r="B50" s="6">
+        <v>3424</v>
+      </c>
+      <c r="C50" s="5">
+        <v>6245</v>
+      </c>
+      <c r="D50" s="7">
+        <v>2509</v>
       </c>
       <c r="E50" s="7">
-        <v>1164</v>
+        <v>1181</v>
       </c>
       <c r="F50" s="8">
-        <v>424</v>
+        <v>639</v>
       </c>
       <c r="G50" s="8">
-        <v>629</v>
+        <v>426</v>
       </c>
       <c r="H50" s="8">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="I50" s="8">
         <v>31</v>
@@ -3353,33 +3351,33 @@
         <v>12</v>
       </c>
       <c r="O50" s="8">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P50" s="8">
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="5">
+      <c r="B51" s="6">
         <v>1844</v>
       </c>
-      <c r="C51" s="6">
+      <c r="C51" s="5">
         <v>1846</v>
       </c>
       <c r="D51" s="8">
         <v>472</v>
       </c>
-      <c r="E51" s="10">
+      <c r="E51" s="8">
         <v>676</v>
       </c>
       <c r="F51" s="8">
+        <v>267</v>
+      </c>
+      <c r="G51" s="8">
         <v>193</v>
-      </c>
-      <c r="G51" s="8">
-        <v>267</v>
       </c>
       <c r="H51" s="8">
         <v>214</v>
@@ -3409,27 +3407,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="52" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B52" s="5">
+      <c r="B52" s="6">
         <v>4314</v>
       </c>
-      <c r="C52" s="6">
+      <c r="C52" s="5">
         <v>8031</v>
       </c>
-      <c r="D52" s="5">
+      <c r="D52" s="7">
         <v>2438</v>
       </c>
       <c r="E52" s="7">
         <v>1484</v>
       </c>
       <c r="F52" s="8">
+        <v>585</v>
+      </c>
+      <c r="G52" s="8">
         <v>388</v>
-      </c>
-      <c r="G52" s="8">
-        <v>585</v>
       </c>
       <c r="H52" s="8">
         <v>88</v>
@@ -3459,27 +3457,27 @@
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B53" s="8">
-        <v>180</v>
+      <c r="B53" s="10">
+        <v>184</v>
       </c>
       <c r="C53" s="9">
-        <v>815</v>
+        <v>821</v>
       </c>
       <c r="D53" s="8">
         <v>181</v>
       </c>
-      <c r="E53" s="10">
-        <v>27</v>
+      <c r="E53" s="8">
+        <v>28</v>
       </c>
       <c r="F53" s="8">
+        <v>15</v>
+      </c>
+      <c r="G53" s="8">
         <v>9</v>
-      </c>
-      <c r="G53" s="8">
-        <v>15</v>
       </c>
       <c r="H53" s="8">
         <v>11</v>
@@ -3488,7 +3486,7 @@
         <v>3</v>
       </c>
       <c r="J53" s="8">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K53" s="8">
         <v>3</v>
@@ -3509,27 +3507,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B54" s="5">
-        <v>1228</v>
-      </c>
-      <c r="C54" s="6">
-        <v>2510</v>
+      <c r="B54" s="6">
+        <v>1233</v>
+      </c>
+      <c r="C54" s="5">
+        <v>2520</v>
       </c>
       <c r="D54" s="8">
         <v>955</v>
       </c>
-      <c r="E54" s="10">
-        <v>329</v>
+      <c r="E54" s="8">
+        <v>333</v>
       </c>
       <c r="F54" s="8">
+        <v>170</v>
+      </c>
+      <c r="G54" s="8">
         <v>169</v>
-      </c>
-      <c r="G54" s="8">
-        <v>170</v>
       </c>
       <c r="H54" s="8">
         <v>53</v>
@@ -3559,27 +3557,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="55" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B55" s="5">
-        <v>1200</v>
-      </c>
-      <c r="C55" s="6">
-        <v>3528</v>
-      </c>
-      <c r="D55" s="5">
+      <c r="B55" s="6">
+        <v>1201</v>
+      </c>
+      <c r="C55" s="5">
+        <v>3539</v>
+      </c>
+      <c r="D55" s="7">
         <v>1024</v>
       </c>
-      <c r="E55" s="10">
-        <v>225</v>
+      <c r="E55" s="8">
+        <v>228</v>
       </c>
       <c r="F55" s="8">
+        <v>79</v>
+      </c>
+      <c r="G55" s="8">
         <v>112</v>
-      </c>
-      <c r="G55" s="8">
-        <v>79</v>
       </c>
       <c r="H55" s="8">
         <v>45</v>
@@ -3609,27 +3607,27 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B56" s="5">
-        <v>1231</v>
-      </c>
-      <c r="C56" s="6">
-        <v>2883</v>
-      </c>
-      <c r="D56" s="5">
-        <v>1037</v>
-      </c>
-      <c r="E56" s="10">
-        <v>371</v>
+      <c r="B56" s="6">
+        <v>1244</v>
+      </c>
+      <c r="C56" s="5">
+        <v>2896</v>
+      </c>
+      <c r="D56" s="7">
+        <v>1040</v>
+      </c>
+      <c r="E56" s="8">
+        <v>373</v>
       </c>
       <c r="F56" s="8">
+        <v>207</v>
+      </c>
+      <c r="G56" s="8">
         <v>140</v>
-      </c>
-      <c r="G56" s="8">
-        <v>201</v>
       </c>
       <c r="H56" s="8">
         <v>71</v>
@@ -3659,27 +3657,27 @@
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="8">
-        <v>735</v>
-      </c>
-      <c r="C57" s="6">
-        <v>1437</v>
+      <c r="B57" s="10">
+        <v>739</v>
+      </c>
+      <c r="C57" s="5">
+        <v>1445</v>
       </c>
       <c r="D57" s="8">
-        <v>454</v>
-      </c>
-      <c r="E57" s="10">
-        <v>300</v>
+        <v>460</v>
+      </c>
+      <c r="E57" s="8">
+        <v>304</v>
       </c>
       <c r="F57" s="8">
+        <v>172</v>
+      </c>
+      <c r="G57" s="8">
         <v>158</v>
-      </c>
-      <c r="G57" s="8">
-        <v>171</v>
       </c>
       <c r="H57" s="8">
         <v>205</v>
@@ -3709,36 +3707,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>72</v>
       </c>
       <c r="B58" s="11">
-        <v>1277</v>
-      </c>
-      <c r="C58" s="5">
-        <v>1062</v>
+        <v>1295</v>
+      </c>
+      <c r="C58" s="7">
+        <v>1066</v>
       </c>
       <c r="D58" s="8">
-        <v>312</v>
-      </c>
-      <c r="E58" s="10">
-        <v>478</v>
+        <v>314</v>
+      </c>
+      <c r="E58" s="8">
+        <v>481</v>
       </c>
       <c r="F58" s="8">
+        <v>109</v>
+      </c>
+      <c r="G58" s="8">
         <v>166</v>
       </c>
-      <c r="G58" s="8">
-        <v>109</v>
-      </c>
       <c r="H58" s="8">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="I58" s="8">
         <v>9</v>
       </c>
       <c r="J58" s="8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K58" s="8">
         <v>18</v>
@@ -3759,27 +3757,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B59" s="8">
+      <c r="B59" s="10">
         <v>437</v>
       </c>
-      <c r="C59" s="6">
+      <c r="C59" s="5">
         <v>2127</v>
       </c>
       <c r="D59" s="8">
         <v>399</v>
       </c>
-      <c r="E59" s="10">
+      <c r="E59" s="8">
         <v>130</v>
       </c>
       <c r="F59" s="8">
+        <v>37</v>
+      </c>
+      <c r="G59" s="8">
         <v>70</v>
-      </c>
-      <c r="G59" s="8">
-        <v>37</v>
       </c>
       <c r="H59" s="8">
         <v>33</v>
@@ -3809,27 +3807,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="8">
-        <v>870</v>
-      </c>
-      <c r="C60" s="6">
-        <v>1316</v>
+      <c r="B60" s="10">
+        <v>871</v>
+      </c>
+      <c r="C60" s="5">
+        <v>1317</v>
       </c>
       <c r="D60" s="8">
         <v>306</v>
       </c>
-      <c r="E60" s="10">
+      <c r="E60" s="8">
         <v>280</v>
       </c>
       <c r="F60" s="8">
+        <v>105</v>
+      </c>
+      <c r="G60" s="8">
         <v>92</v>
-      </c>
-      <c r="G60" s="8">
-        <v>103</v>
       </c>
       <c r="H60" s="8">
         <v>160</v>
@@ -3859,27 +3857,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B61" s="5">
+      <c r="B61" s="6">
         <v>39269</v>
       </c>
-      <c r="C61" s="6">
+      <c r="C61" s="5">
         <v>72323</v>
       </c>
-      <c r="D61" s="5">
+      <c r="D61" s="7">
         <v>22227</v>
       </c>
       <c r="E61" s="7">
         <v>16426</v>
       </c>
-      <c r="F61" s="5">
+      <c r="F61" s="7">
+        <v>5421</v>
+      </c>
+      <c r="G61" s="7">
         <v>2771</v>
-      </c>
-      <c r="G61" s="5">
-        <v>5421</v>
       </c>
       <c r="H61" s="8">
         <v>861</v>
@@ -3909,27 +3907,27 @@
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>76</v>
       </c>
       <c r="B62" s="12">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="C62" s="8">
         <v>266</v>
       </c>
       <c r="D62" s="8">
-        <v>72</v>
-      </c>
-      <c r="E62" s="10">
-        <v>124</v>
+        <v>73</v>
+      </c>
+      <c r="E62" s="8">
+        <v>128</v>
       </c>
       <c r="F62" s="8">
+        <v>19</v>
+      </c>
+      <c r="G62" s="8">
         <v>36</v>
-      </c>
-      <c r="G62" s="8">
-        <v>19</v>
       </c>
       <c r="H62" s="8">
         <v>30</v>
@@ -3959,27 +3957,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B63" s="8">
-        <v>412</v>
-      </c>
-      <c r="C63" s="6">
-        <v>1310</v>
+      <c r="B63" s="10">
+        <v>416</v>
+      </c>
+      <c r="C63" s="5">
+        <v>1320</v>
       </c>
       <c r="D63" s="8">
-        <v>373</v>
-      </c>
-      <c r="E63" s="10">
-        <v>119</v>
+        <v>374</v>
+      </c>
+      <c r="E63" s="8">
+        <v>121</v>
       </c>
       <c r="F63" s="8">
+        <v>46</v>
+      </c>
+      <c r="G63" s="8">
         <v>62</v>
-      </c>
-      <c r="G63" s="8">
-        <v>46</v>
       </c>
       <c r="H63" s="8">
         <v>29</v>
@@ -4009,27 +4007,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="B64" s="5">
-        <v>1595</v>
-      </c>
-      <c r="C64" s="6">
-        <v>4860</v>
-      </c>
-      <c r="D64" s="5">
-        <v>1824</v>
-      </c>
-      <c r="E64" s="10">
-        <v>777</v>
+      <c r="B64" s="6">
+        <v>1610</v>
+      </c>
+      <c r="C64" s="5">
+        <v>4896</v>
+      </c>
+      <c r="D64" s="7">
+        <v>1833</v>
+      </c>
+      <c r="E64" s="8">
+        <v>782</v>
       </c>
       <c r="F64" s="8">
-        <v>231</v>
+        <v>336</v>
       </c>
       <c r="G64" s="8">
-        <v>334</v>
+        <v>233</v>
       </c>
       <c r="H64" s="8">
         <v>42</v>
@@ -4059,27 +4057,27 @@
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B65" s="5">
+      <c r="B65" s="6">
         <v>2116</v>
       </c>
-      <c r="C65" s="6">
+      <c r="C65" s="5">
         <v>6506</v>
       </c>
-      <c r="D65" s="5">
+      <c r="D65" s="7">
         <v>1998</v>
       </c>
-      <c r="E65" s="10">
+      <c r="E65" s="8">
         <v>474</v>
       </c>
       <c r="F65" s="8">
+        <v>137</v>
+      </c>
+      <c r="G65" s="8">
         <v>228</v>
-      </c>
-      <c r="G65" s="8">
-        <v>137</v>
       </c>
       <c r="H65" s="8">
         <v>66</v>
@@ -4109,27 +4107,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B66" s="5">
-        <v>9002</v>
-      </c>
-      <c r="C66" s="6">
-        <v>12220</v>
-      </c>
-      <c r="D66" s="5">
-        <v>5128</v>
+      <c r="B66" s="6">
+        <v>9165</v>
+      </c>
+      <c r="C66" s="5">
+        <v>12332</v>
+      </c>
+      <c r="D66" s="7">
+        <v>5173</v>
       </c>
       <c r="E66" s="7">
-        <v>3492</v>
-      </c>
-      <c r="F66" s="8">
-        <v>965</v>
-      </c>
-      <c r="G66" s="5">
-        <v>1627</v>
+        <v>3540</v>
+      </c>
+      <c r="F66" s="7">
+        <v>1641</v>
+      </c>
+      <c r="G66" s="8">
+        <v>979</v>
       </c>
       <c r="H66" s="8">
         <v>174</v>
@@ -4141,7 +4139,7 @@
         <v>150</v>
       </c>
       <c r="K66" s="8">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L66" s="8">
         <v>7</v>
@@ -4156,30 +4154,30 @@
         <v>23</v>
       </c>
       <c r="P66" s="8">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B67" s="8">
-        <v>494</v>
-      </c>
-      <c r="C67" s="6">
-        <v>2650</v>
+      <c r="B67" s="10">
+        <v>499</v>
+      </c>
+      <c r="C67" s="5">
+        <v>2656</v>
       </c>
       <c r="D67" s="8">
-        <v>504</v>
-      </c>
-      <c r="E67" s="10">
+        <v>505</v>
+      </c>
+      <c r="E67" s="8">
         <v>126</v>
       </c>
       <c r="F67" s="8">
+        <v>46</v>
+      </c>
+      <c r="G67" s="8">
         <v>83</v>
-      </c>
-      <c r="G67" s="8">
-        <v>46</v>
       </c>
       <c r="H67" s="8">
         <v>23</v>
@@ -4209,30 +4207,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B68" s="5">
-        <v>1982</v>
-      </c>
-      <c r="C68" s="6">
-        <v>4918</v>
-      </c>
-      <c r="D68" s="5">
-        <v>1165</v>
-      </c>
-      <c r="E68" s="10">
-        <v>599</v>
+      <c r="B68" s="6">
+        <v>2021</v>
+      </c>
+      <c r="C68" s="5">
+        <v>4972</v>
+      </c>
+      <c r="D68" s="7">
+        <v>1173</v>
+      </c>
+      <c r="E68" s="8">
+        <v>605</v>
       </c>
       <c r="F68" s="8">
+        <v>201</v>
+      </c>
+      <c r="G68" s="8">
         <v>137</v>
       </c>
-      <c r="G68" s="8">
-        <v>199</v>
-      </c>
       <c r="H68" s="8">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I68" s="8">
         <v>18</v>
@@ -4241,7 +4239,7 @@
         <v>36</v>
       </c>
       <c r="K68" s="8">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="L68" s="8">
         <v>4</v>
@@ -4259,27 +4257,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="B69" s="5">
+      <c r="B69" s="6">
         <v>12602</v>
       </c>
-      <c r="C69" s="6">
+      <c r="C69" s="5">
         <v>12956</v>
       </c>
-      <c r="D69" s="5">
+      <c r="D69" s="7">
         <v>4537</v>
       </c>
       <c r="E69" s="7">
         <v>10199</v>
       </c>
-      <c r="F69" s="5">
+      <c r="F69" s="7">
+        <v>1800</v>
+      </c>
+      <c r="G69" s="7">
         <v>1330</v>
-      </c>
-      <c r="G69" s="5">
-        <v>1800</v>
       </c>
       <c r="H69" s="8">
         <v>95</v>
@@ -4309,36 +4307,36 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B70" s="8">
-        <v>212</v>
+      <c r="B70" s="10">
+        <v>213</v>
       </c>
       <c r="C70" s="9">
-        <v>933</v>
+        <v>948</v>
       </c>
       <c r="D70" s="8">
-        <v>272</v>
-      </c>
-      <c r="E70" s="10">
-        <v>81</v>
+        <v>274</v>
+      </c>
+      <c r="E70" s="8">
+        <v>83</v>
       </c>
       <c r="F70" s="8">
+        <v>54</v>
+      </c>
+      <c r="G70" s="8">
         <v>57</v>
       </c>
-      <c r="G70" s="8">
-        <v>52</v>
-      </c>
       <c r="H70" s="8">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="I70" s="8">
         <v>6</v>
       </c>
       <c r="J70" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K70" s="8">
         <v>5</v>
@@ -4347,10 +4345,10 @@
         <v>3</v>
       </c>
       <c r="M70" s="8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N70" s="8">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="O70" s="8">
         <v>5</v>
@@ -4359,27 +4357,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="B71" s="8">
+      <c r="B71" s="10">
         <v>649</v>
       </c>
-      <c r="C71" s="6">
+      <c r="C71" s="5">
         <v>2393</v>
       </c>
       <c r="D71" s="8">
         <v>626</v>
       </c>
-      <c r="E71" s="10">
+      <c r="E71" s="8">
         <v>182</v>
       </c>
       <c r="F71" s="8">
+        <v>88</v>
+      </c>
+      <c r="G71" s="8">
         <v>96</v>
-      </c>
-      <c r="G71" s="8">
-        <v>88</v>
       </c>
       <c r="H71" s="8">
         <v>22</v>
@@ -4409,27 +4407,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="B72" s="5">
-        <v>1177</v>
-      </c>
-      <c r="C72" s="6">
-        <v>2495</v>
+      <c r="B72" s="6">
+        <v>1191</v>
+      </c>
+      <c r="C72" s="5">
+        <v>2513</v>
       </c>
       <c r="D72" s="8">
-        <v>859</v>
-      </c>
-      <c r="E72" s="10">
-        <v>391</v>
+        <v>861</v>
+      </c>
+      <c r="E72" s="8">
+        <v>392</v>
       </c>
       <c r="F72" s="8">
+        <v>221</v>
+      </c>
+      <c r="G72" s="8">
         <v>139</v>
-      </c>
-      <c r="G72" s="8">
-        <v>219</v>
       </c>
       <c r="H72" s="8">
         <v>41</v>
@@ -4459,11 +4457,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="B73" s="8">
+      <c r="B73" s="10">
         <v>174</v>
       </c>
       <c r="C73" s="9">
@@ -4472,14 +4470,14 @@
       <c r="D73" s="8">
         <v>259</v>
       </c>
-      <c r="E73" s="10">
+      <c r="E73" s="8">
         <v>58</v>
       </c>
       <c r="F73" s="8">
+        <v>31</v>
+      </c>
+      <c r="G73" s="8">
         <v>54</v>
-      </c>
-      <c r="G73" s="8">
-        <v>31</v>
       </c>
       <c r="H73" s="8">
         <v>12</v>
@@ -4509,27 +4507,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="74" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B74" s="8">
-        <v>773</v>
-      </c>
-      <c r="C74" s="6">
-        <v>2320</v>
+      <c r="B74" s="10">
+        <v>777</v>
+      </c>
+      <c r="C74" s="5">
+        <v>2329</v>
       </c>
       <c r="D74" s="8">
         <v>654</v>
       </c>
-      <c r="E74" s="10">
-        <v>291</v>
+      <c r="E74" s="8">
+        <v>293</v>
       </c>
       <c r="F74" s="8">
+        <v>80</v>
+      </c>
+      <c r="G74" s="8">
         <v>106</v>
-      </c>
-      <c r="G74" s="8">
-        <v>79</v>
       </c>
       <c r="H74" s="8">
         <v>42</v>
@@ -4559,30 +4557,30 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="B75" s="5">
-        <v>5000</v>
-      </c>
-      <c r="C75" s="6">
-        <v>10211</v>
-      </c>
-      <c r="D75" s="5">
-        <v>2619</v>
+      <c r="B75" s="6">
+        <v>5105</v>
+      </c>
+      <c r="C75" s="5">
+        <v>10329</v>
+      </c>
+      <c r="D75" s="7">
+        <v>2639</v>
       </c>
       <c r="E75" s="7">
-        <v>1537</v>
+        <v>1554</v>
       </c>
       <c r="F75" s="8">
-        <v>453</v>
+        <v>602</v>
       </c>
       <c r="G75" s="8">
-        <v>601</v>
+        <v>454</v>
       </c>
       <c r="H75" s="8">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="I75" s="8">
         <v>38</v>
@@ -4603,33 +4601,33 @@
         <v>8</v>
       </c>
       <c r="O75" s="8">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="P75" s="8">
         <v>27</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="B76" s="8">
-        <v>519</v>
-      </c>
-      <c r="C76" s="6">
-        <v>1063</v>
+      <c r="B76" s="10">
+        <v>521</v>
+      </c>
+      <c r="C76" s="5">
+        <v>1066</v>
       </c>
       <c r="D76" s="8">
-        <v>297</v>
-      </c>
-      <c r="E76" s="10">
-        <v>281</v>
+        <v>299</v>
+      </c>
+      <c r="E76" s="8">
+        <v>284</v>
       </c>
       <c r="F76" s="8">
+        <v>132</v>
+      </c>
+      <c r="G76" s="8">
         <v>106</v>
-      </c>
-      <c r="G76" s="8">
-        <v>130</v>
       </c>
       <c r="H76" s="8">
         <v>96</v>
@@ -4659,27 +4657,27 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="B77" s="5">
-        <v>1721</v>
-      </c>
-      <c r="C77" s="6">
-        <v>2778</v>
-      </c>
-      <c r="D77" s="5">
-        <v>1077</v>
-      </c>
-      <c r="E77" s="10">
-        <v>496</v>
+      <c r="B77" s="6">
+        <v>1734</v>
+      </c>
+      <c r="C77" s="5">
+        <v>2788</v>
+      </c>
+      <c r="D77" s="7">
+        <v>1083</v>
+      </c>
+      <c r="E77" s="8">
+        <v>500</v>
       </c>
       <c r="F77" s="8">
+        <v>223</v>
+      </c>
+      <c r="G77" s="8">
         <v>171</v>
-      </c>
-      <c r="G77" s="8">
-        <v>221</v>
       </c>
       <c r="H77" s="8">
         <v>33</v>
@@ -4697,7 +4695,7 @@
         <v>6</v>
       </c>
       <c r="M77" s="8">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="N77" s="8">
         <v>11</v>
@@ -4709,27 +4707,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="B78" s="8">
+      <c r="B78" s="10">
         <v>692</v>
       </c>
-      <c r="C78" s="6">
+      <c r="C78" s="5">
         <v>2639</v>
       </c>
       <c r="D78" s="8">
         <v>691</v>
       </c>
-      <c r="E78" s="10">
+      <c r="E78" s="8">
         <v>174</v>
       </c>
       <c r="F78" s="8">
+        <v>72</v>
+      </c>
+      <c r="G78" s="8">
         <v>85</v>
-      </c>
-      <c r="G78" s="8">
-        <v>72</v>
       </c>
       <c r="H78" s="8">
         <v>58</v>
@@ -4759,27 +4757,27 @@
         <v>14</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B79" s="5">
+      <c r="B79" s="6">
         <v>2366</v>
       </c>
-      <c r="C79" s="6">
+      <c r="C79" s="5">
         <v>6361</v>
       </c>
-      <c r="D79" s="5">
+      <c r="D79" s="7">
         <v>1376</v>
       </c>
-      <c r="E79" s="10">
+      <c r="E79" s="8">
         <v>534</v>
       </c>
       <c r="F79" s="8">
+        <v>135</v>
+      </c>
+      <c r="G79" s="8">
         <v>261</v>
-      </c>
-      <c r="G79" s="8">
-        <v>135</v>
       </c>
       <c r="H79" s="8">
         <v>855</v>
@@ -4809,27 +4807,27 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="B80" s="5">
-        <v>1491</v>
-      </c>
-      <c r="C80" s="6">
-        <v>3545</v>
-      </c>
-      <c r="D80" s="5">
-        <v>1547</v>
-      </c>
-      <c r="E80" s="10">
-        <v>353</v>
+      <c r="B80" s="6">
+        <v>1506</v>
+      </c>
+      <c r="C80" s="5">
+        <v>3571</v>
+      </c>
+      <c r="D80" s="7">
+        <v>1551</v>
+      </c>
+      <c r="E80" s="8">
+        <v>360</v>
       </c>
       <c r="F80" s="8">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G80" s="8">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="H80" s="8">
         <v>44</v>
@@ -4856,42 +4854,42 @@
         <v>9</v>
       </c>
       <c r="P80" s="8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="B81" s="5">
-        <v>2379</v>
-      </c>
-      <c r="C81" s="6">
-        <v>4776</v>
-      </c>
-      <c r="D81" s="5">
-        <v>1501</v>
-      </c>
-      <c r="E81" s="10">
-        <v>655</v>
+      <c r="B81" s="6">
+        <v>2393</v>
+      </c>
+      <c r="C81" s="5">
+        <v>4799</v>
+      </c>
+      <c r="D81" s="7">
+        <v>1507</v>
+      </c>
+      <c r="E81" s="8">
+        <v>662</v>
       </c>
       <c r="F81" s="8">
+        <v>298</v>
+      </c>
+      <c r="G81" s="8">
         <v>226</v>
-      </c>
-      <c r="G81" s="8">
-        <v>292</v>
       </c>
       <c r="H81" s="8">
         <v>102</v>
       </c>
       <c r="I81" s="8">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J81" s="8">
         <v>59</v>
       </c>
       <c r="K81" s="8">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L81" s="8">
         <v>11</v>
@@ -4909,30 +4907,30 @@
         <v>14</v>
       </c>
     </row>
-    <row r="82" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="B82" s="5">
-        <v>1137</v>
-      </c>
-      <c r="C82" s="6">
-        <v>2145</v>
+      <c r="B82" s="6">
+        <v>1146</v>
+      </c>
+      <c r="C82" s="5">
+        <v>2153</v>
       </c>
       <c r="D82" s="8">
-        <v>400</v>
-      </c>
-      <c r="E82" s="10">
-        <v>273</v>
+        <v>403</v>
+      </c>
+      <c r="E82" s="8">
+        <v>276</v>
       </c>
       <c r="F82" s="8">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="G82" s="8">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="H82" s="8">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="I82" s="8">
         <v>3</v>
@@ -4941,7 +4939,7 @@
         <v>37</v>
       </c>
       <c r="K82" s="8">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L82" s="8">
         <v>1</v>
@@ -4959,27 +4957,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="B83" s="8">
+      <c r="B83" s="10">
         <v>861</v>
       </c>
-      <c r="C83" s="6">
+      <c r="C83" s="5">
         <v>2829</v>
       </c>
       <c r="D83" s="8">
         <v>817</v>
       </c>
-      <c r="E83" s="10">
+      <c r="E83" s="8">
         <v>213</v>
       </c>
       <c r="F83" s="8">
+        <v>53</v>
+      </c>
+      <c r="G83" s="8">
         <v>62</v>
-      </c>
-      <c r="G83" s="8">
-        <v>53</v>
       </c>
       <c r="H83" s="8">
         <v>27</v>
@@ -5009,27 +5007,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="84" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="B84" s="8">
-        <v>525</v>
-      </c>
-      <c r="C84" s="6">
-        <v>2068</v>
+      <c r="B84" s="10">
+        <v>529</v>
+      </c>
+      <c r="C84" s="5">
+        <v>2075</v>
       </c>
       <c r="D84" s="8">
-        <v>325</v>
-      </c>
-      <c r="E84" s="10">
-        <v>153</v>
+        <v>330</v>
+      </c>
+      <c r="E84" s="8">
+        <v>155</v>
       </c>
       <c r="F84" s="8">
+        <v>65</v>
+      </c>
+      <c r="G84" s="8">
         <v>95</v>
-      </c>
-      <c r="G84" s="8">
-        <v>65</v>
       </c>
       <c r="H84" s="8">
         <v>212</v>
@@ -5059,27 +5057,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="85" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="B85" s="8">
-        <v>719</v>
-      </c>
-      <c r="C85" s="6">
-        <v>1757</v>
+      <c r="B85" s="10">
+        <v>740</v>
+      </c>
+      <c r="C85" s="5">
+        <v>1775</v>
       </c>
       <c r="D85" s="8">
-        <v>532</v>
-      </c>
-      <c r="E85" s="10">
-        <v>220</v>
+        <v>537</v>
+      </c>
+      <c r="E85" s="8">
+        <v>223</v>
       </c>
       <c r="F85" s="8">
+        <v>101</v>
+      </c>
+      <c r="G85" s="8">
         <v>89</v>
-      </c>
-      <c r="G85" s="8">
-        <v>101</v>
       </c>
       <c r="H85" s="8">
         <v>58</v>
@@ -5109,27 +5107,27 @@
         <v>8</v>
       </c>
     </row>
-    <row r="86" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="B86" s="8">
+      <c r="B86" s="10">
         <v>671</v>
       </c>
-      <c r="C86" s="6">
+      <c r="C86" s="5">
         <v>1211</v>
       </c>
       <c r="D86" s="8">
         <v>533</v>
       </c>
-      <c r="E86" s="10">
+      <c r="E86" s="8">
         <v>174</v>
       </c>
       <c r="F86" s="8">
+        <v>92</v>
+      </c>
+      <c r="G86" s="8">
         <v>74</v>
-      </c>
-      <c r="G86" s="8">
-        <v>92</v>
       </c>
       <c r="H86" s="8">
         <v>38</v>
@@ -5159,27 +5157,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="B87" s="5">
-        <v>1003</v>
-      </c>
-      <c r="C87" s="6">
-        <v>1941</v>
+      <c r="B87" s="6">
+        <v>1021</v>
+      </c>
+      <c r="C87" s="5">
+        <v>1949</v>
       </c>
       <c r="D87" s="8">
-        <v>822</v>
-      </c>
-      <c r="E87" s="10">
-        <v>302</v>
+        <v>827</v>
+      </c>
+      <c r="E87" s="8">
+        <v>305</v>
       </c>
       <c r="F87" s="8">
+        <v>119</v>
+      </c>
+      <c r="G87" s="8">
         <v>147</v>
-      </c>
-      <c r="G87" s="8">
-        <v>119</v>
       </c>
       <c r="H87" s="8">
         <v>42</v>
@@ -5209,27 +5207,27 @@
         <v>5</v>
       </c>
     </row>
-    <row r="88" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B88" s="8">
-        <v>468</v>
+      <c r="B88" s="10">
+        <v>470</v>
       </c>
       <c r="C88" s="9">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="D88" s="8">
-        <v>160</v>
-      </c>
-      <c r="E88" s="10">
+        <v>161</v>
+      </c>
+      <c r="E88" s="8">
         <v>111</v>
       </c>
       <c r="F88" s="8">
+        <v>64</v>
+      </c>
+      <c r="G88" s="8">
         <v>58</v>
-      </c>
-      <c r="G88" s="8">
-        <v>63</v>
       </c>
       <c r="H88" s="8">
         <v>82</v>
@@ -5259,27 +5257,27 @@
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B89" s="5">
-        <v>1276</v>
-      </c>
-      <c r="C89" s="6">
-        <v>1879</v>
+      <c r="B89" s="6">
+        <v>1288</v>
+      </c>
+      <c r="C89" s="5">
+        <v>1890</v>
       </c>
       <c r="D89" s="8">
-        <v>549</v>
-      </c>
-      <c r="E89" s="10">
-        <v>685</v>
+        <v>552</v>
+      </c>
+      <c r="E89" s="8">
+        <v>692</v>
       </c>
       <c r="F89" s="8">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="G89" s="8">
-        <v>296</v>
+        <v>304</v>
       </c>
       <c r="H89" s="8">
         <v>148</v>
@@ -5309,27 +5307,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B90" s="8">
-        <v>88</v>
+      <c r="B90" s="10">
+        <v>91</v>
       </c>
       <c r="C90" s="9">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="D90" s="8">
-        <v>97</v>
-      </c>
-      <c r="E90" s="10">
-        <v>21</v>
+        <v>99</v>
+      </c>
+      <c r="E90" s="8">
+        <v>22</v>
       </c>
       <c r="F90" s="8">
+        <v>15</v>
+      </c>
+      <c r="G90" s="8">
         <v>20</v>
-      </c>
-      <c r="G90" s="8">
-        <v>15</v>
       </c>
       <c r="H90" s="8">
         <v>4</v>
@@ -5359,27 +5357,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B91" s="5">
-        <v>4534</v>
-      </c>
-      <c r="C91" s="6">
-        <v>9053</v>
-      </c>
-      <c r="D91" s="5">
-        <v>3056</v>
+      <c r="B91" s="6">
+        <v>4587</v>
+      </c>
+      <c r="C91" s="5">
+        <v>9117</v>
+      </c>
+      <c r="D91" s="7">
+        <v>3069</v>
       </c>
       <c r="E91" s="7">
-        <v>1748</v>
+        <v>1767</v>
       </c>
       <c r="F91" s="8">
-        <v>503</v>
+        <v>844</v>
       </c>
       <c r="G91" s="8">
-        <v>836</v>
+        <v>506</v>
       </c>
       <c r="H91" s="8">
         <v>157</v>
@@ -5391,13 +5389,13 @@
         <v>103</v>
       </c>
       <c r="K91" s="8">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="L91" s="8">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="M91" s="8">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="N91" s="8">
         <v>11</v>
@@ -5406,30 +5404,30 @@
         <v>19</v>
       </c>
       <c r="P91" s="8">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B92" s="8">
-        <v>793</v>
-      </c>
-      <c r="C92" s="6">
-        <v>3340</v>
+      <c r="B92" s="10">
+        <v>794</v>
+      </c>
+      <c r="C92" s="5">
+        <v>3348</v>
       </c>
       <c r="D92" s="8">
-        <v>764</v>
-      </c>
-      <c r="E92" s="10">
+        <v>768</v>
+      </c>
+      <c r="E92" s="8">
         <v>217</v>
       </c>
       <c r="F92" s="8">
+        <v>58</v>
+      </c>
+      <c r="G92" s="8">
         <v>87</v>
-      </c>
-      <c r="G92" s="8">
-        <v>58</v>
       </c>
       <c r="H92" s="8">
         <v>36</v>
@@ -5459,77 +5457,77 @@
         <v>11</v>
       </c>
     </row>
-    <row r="93" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B93" s="5">
-        <v>49980</v>
-      </c>
-      <c r="C93" s="6">
-        <v>78225</v>
-      </c>
-      <c r="D93" s="5">
-        <v>23361</v>
+      <c r="B93" s="6">
+        <v>50919</v>
+      </c>
+      <c r="C93" s="5">
+        <v>79007</v>
+      </c>
+      <c r="D93" s="7">
+        <v>23544</v>
       </c>
       <c r="E93" s="7">
-        <v>27511</v>
-      </c>
-      <c r="F93" s="5">
-        <v>3724</v>
-      </c>
-      <c r="G93" s="5">
-        <v>6764</v>
+        <v>27837</v>
+      </c>
+      <c r="F93" s="7">
+        <v>6821</v>
+      </c>
+      <c r="G93" s="7">
+        <v>3759</v>
       </c>
       <c r="H93" s="8">
         <v>505</v>
       </c>
       <c r="I93" s="8">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="J93" s="8">
-        <v>807</v>
+        <v>812</v>
       </c>
       <c r="K93" s="8">
-        <v>398</v>
+        <v>403</v>
       </c>
       <c r="L93" s="8">
         <v>51</v>
       </c>
       <c r="M93" s="8">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="N93" s="8">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="O93" s="8">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="P93" s="8">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B94" s="8">
-        <v>546</v>
-      </c>
-      <c r="C94" s="6">
-        <v>2206</v>
+      <c r="B94" s="10">
+        <v>548</v>
+      </c>
+      <c r="C94" s="5">
+        <v>2211</v>
       </c>
       <c r="D94" s="8">
-        <v>479</v>
-      </c>
-      <c r="E94" s="10">
+        <v>480</v>
+      </c>
+      <c r="E94" s="8">
         <v>132</v>
       </c>
       <c r="F94" s="8">
+        <v>46</v>
+      </c>
+      <c r="G94" s="8">
         <v>68</v>
-      </c>
-      <c r="G94" s="8">
-        <v>46</v>
       </c>
       <c r="H94" s="8">
         <v>22</v>
@@ -5559,27 +5557,27 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>108</v>
       </c>
-      <c r="B95" s="8">
+      <c r="B95" s="10">
         <v>291</v>
       </c>
-      <c r="C95" s="6">
+      <c r="C95" s="5">
         <v>1078</v>
       </c>
       <c r="D95" s="8">
         <v>268</v>
       </c>
-      <c r="E95" s="10">
+      <c r="E95" s="8">
         <v>56</v>
       </c>
       <c r="F95" s="8">
+        <v>13</v>
+      </c>
+      <c r="G95" s="8">
         <v>43</v>
-      </c>
-      <c r="G95" s="8">
-        <v>13</v>
       </c>
       <c r="H95" s="8">
         <v>37</v>
@@ -5609,30 +5607,30 @@
         <v>4</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B96" s="11">
-        <v>4516</v>
-      </c>
-      <c r="C96" s="5">
-        <v>2236</v>
+        <v>4708</v>
+      </c>
+      <c r="C96" s="7">
+        <v>2298</v>
       </c>
       <c r="D96" s="8">
-        <v>704</v>
+        <v>716</v>
       </c>
       <c r="E96" s="7">
-        <v>1303</v>
+        <v>1336</v>
       </c>
       <c r="F96" s="8">
-        <v>240</v>
+        <v>469</v>
       </c>
       <c r="G96" s="8">
-        <v>469</v>
+        <v>245</v>
       </c>
       <c r="H96" s="8">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I96" s="8">
         <v>8</v>
@@ -5641,7 +5639,7 @@
         <v>37</v>
       </c>
       <c r="K96" s="8">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L96" s="8">
         <v>1</v>
@@ -5659,27 +5657,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="97" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B97" s="5">
+      <c r="B97" s="6">
         <v>2329</v>
       </c>
-      <c r="C97" s="6">
+      <c r="C97" s="5">
         <v>5752</v>
       </c>
-      <c r="D97" s="5">
+      <c r="D97" s="7">
         <v>1668</v>
       </c>
-      <c r="E97" s="10">
+      <c r="E97" s="8">
         <v>490</v>
       </c>
       <c r="F97" s="8">
+        <v>206</v>
+      </c>
+      <c r="G97" s="8">
         <v>196</v>
-      </c>
-      <c r="G97" s="8">
-        <v>206</v>
       </c>
       <c r="H97" s="8">
         <v>115</v>
@@ -5709,27 +5707,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="98" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="B98" s="8">
-        <v>868</v>
-      </c>
-      <c r="C98" s="6">
-        <v>1780</v>
+      <c r="B98" s="10">
+        <v>873</v>
+      </c>
+      <c r="C98" s="5">
+        <v>1787</v>
       </c>
       <c r="D98" s="8">
-        <v>632</v>
-      </c>
-      <c r="E98" s="10">
-        <v>246</v>
+        <v>634</v>
+      </c>
+      <c r="E98" s="8">
+        <v>247</v>
       </c>
       <c r="F98" s="8">
+        <v>87</v>
+      </c>
+      <c r="G98" s="8">
         <v>84</v>
-      </c>
-      <c r="G98" s="8">
-        <v>87</v>
       </c>
       <c r="H98" s="8">
         <v>22</v>
@@ -5759,27 +5757,27 @@
         <v>7</v>
       </c>
     </row>
-    <row r="99" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="B99" s="5">
+      <c r="B99" s="6">
         <v>1927</v>
       </c>
-      <c r="C99" s="6">
+      <c r="C99" s="5">
         <v>5052</v>
       </c>
-      <c r="D99" s="5">
+      <c r="D99" s="7">
         <v>1545</v>
       </c>
-      <c r="E99" s="10">
+      <c r="E99" s="8">
         <v>409</v>
       </c>
       <c r="F99" s="8">
+        <v>143</v>
+      </c>
+      <c r="G99" s="8">
         <v>149</v>
-      </c>
-      <c r="G99" s="8">
-        <v>143</v>
       </c>
       <c r="H99" s="8">
         <v>61</v>
@@ -5809,27 +5807,27 @@
         <v>19</v>
       </c>
     </row>
-    <row r="100" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="B100" s="8">
-        <v>451</v>
+      <c r="B100" s="10">
+        <v>461</v>
       </c>
       <c r="C100" s="9">
-        <v>779</v>
+        <v>784</v>
       </c>
       <c r="D100" s="8">
-        <v>300</v>
-      </c>
-      <c r="E100" s="10">
-        <v>118</v>
+        <v>302</v>
+      </c>
+      <c r="E100" s="8">
+        <v>120</v>
       </c>
       <c r="F100" s="8">
+        <v>46</v>
+      </c>
+      <c r="G100" s="8">
         <v>50</v>
-      </c>
-      <c r="G100" s="8">
-        <v>45</v>
       </c>
       <c r="H100" s="8">
         <v>13</v>
@@ -5859,30 +5857,30 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B101" s="8">
-        <v>699</v>
+      <c r="B101" s="10">
+        <v>709</v>
       </c>
       <c r="C101" s="9">
-        <v>842</v>
+        <v>848</v>
       </c>
       <c r="D101" s="8">
         <v>206</v>
       </c>
-      <c r="E101" s="10">
-        <v>314</v>
+      <c r="E101" s="8">
+        <v>318</v>
       </c>
       <c r="F101" s="8">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G101" s="8">
         <v>79</v>
       </c>
       <c r="H101" s="8">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I101" s="8">
         <v>2</v>
@@ -5911,6 +5909,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>